<commit_message>
Clean up codebase: remove AI features, database code, sample recipes, and unused files
</commit_message>
<xml_diff>
--- a/backend/data/bookmarks.xlsx
+++ b/backend/data/bookmarks.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>user_id</t>
   </si>
@@ -23,6 +23,15 @@
   </si>
   <si>
     <t>112140</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>45</t>
   </si>
 </sst>
 </file>
@@ -400,7 +409,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -425,6 +434,50 @@
         <v>45963.812435</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45996.82861790509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45996.84202701389</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45996.85839129629</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45996.858683252314</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Clean up code, fix authentication, update to use recipes.csv, remove unnecessary console logs
</commit_message>
<xml_diff>
--- a/backend/data/bookmarks.xlsx
+++ b/backend/data/bookmarks.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>user_id</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t>45</t>
+  </si>
+  <si>
+    <t>347</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>338</t>
+  </si>
+  <si>
+    <t>204</t>
   </si>
 </sst>
 </file>
@@ -409,7 +421,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -478,6 +490,50 @@
         <v>45996.858683252314</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45998.79088569444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45998.790963645835</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45998.791139733796</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45998.791305023144</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>